<commit_message>
Updated packages in Semis and removed dupes in MSS_PARTS.xlsx
</commit_message>
<xml_diff>
--- a/Data/MSS_PARTS.xlsx
+++ b/Data/MSS_PARTS.xlsx
@@ -4,21 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14130" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14130" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Transistors" sheetId="4" r:id="rId1"/>
-    <sheet name="ICs" sheetId="5" r:id="rId2"/>
-    <sheet name="Diodes" sheetId="9" r:id="rId3"/>
-    <sheet name="Electromechanical" sheetId="6" r:id="rId4"/>
-    <sheet name="Misc" sheetId="8" r:id="rId5"/>
+    <sheet name="ICs" sheetId="5" r:id="rId1"/>
+    <sheet name="Electromechanical" sheetId="6" r:id="rId2"/>
+    <sheet name="Misc" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="367">
   <si>
     <t>CD4052</t>
   </si>
@@ -74,105 +72,9 @@
     <t>Verified</t>
   </si>
   <si>
-    <t>15pF</t>
-  </si>
-  <si>
-    <t>MOSFET</t>
-  </si>
-  <si>
-    <t>NPN</t>
-  </si>
-  <si>
-    <t>MPSA18</t>
-  </si>
-  <si>
-    <t>2N5088</t>
-  </si>
-  <si>
-    <t>JFET</t>
-  </si>
-  <si>
-    <t>J201</t>
-  </si>
-  <si>
-    <t>2N5457</t>
-  </si>
-  <si>
-    <t>2n5458</t>
-  </si>
-  <si>
-    <t>2n5459</t>
-  </si>
-  <si>
-    <t>2n5460</t>
-  </si>
-  <si>
-    <t>2n5461</t>
-  </si>
-  <si>
-    <t>J202</t>
-  </si>
-  <si>
-    <t>2n7000</t>
-  </si>
-  <si>
-    <t>2n7002</t>
-  </si>
-  <si>
-    <t>2N5089</t>
-  </si>
-  <si>
-    <t>2n3904</t>
-  </si>
-  <si>
-    <t>2n3906</t>
-  </si>
-  <si>
-    <t>2n4401</t>
-  </si>
-  <si>
-    <t>2n4402</t>
-  </si>
-  <si>
-    <t>2n5087</t>
-  </si>
-  <si>
-    <t>2n4403</t>
-  </si>
-  <si>
-    <t>MPSA14</t>
-  </si>
-  <si>
-    <t>MPSA63</t>
-  </si>
-  <si>
-    <t>MPSA64</t>
-  </si>
-  <si>
-    <t>2n2222</t>
-  </si>
-  <si>
-    <t>BC560</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>NPN Darlington</t>
-  </si>
-  <si>
-    <t>NPN Darlington Vceo=30V, Ic=1.2A, hfe=10K@10mA</t>
-  </si>
-  <si>
-    <t>NPN Vceo=45V, Ic=200mA, hfe=1150@10mA</t>
-  </si>
-  <si>
-    <t>PNP Darlington</t>
-  </si>
-  <si>
-    <t>PNP Darlington Vceo=-30V, Ic=-500mA, hfe=5k@10mA</t>
-  </si>
-  <si>
     <t>Jack TRS</t>
   </si>
   <si>
@@ -272,90 +174,6 @@
     <t>Dual RCA - Horizontal</t>
   </si>
   <si>
-    <t>PNP Darlington Vceo=-30V, Ic=-500mA, hfe=10K@10mA</t>
-  </si>
-  <si>
-    <t>PNP</t>
-  </si>
-  <si>
-    <t>NPN Vceo=30V, Ic=50mA, hfe=300@10mA</t>
-  </si>
-  <si>
-    <t>PNP Vceo=50V, Ic=50mA, hfe=250@10mA</t>
-  </si>
-  <si>
-    <t>NPN Vceo=25V, Ic=50mA, hfe=400@10mA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPN </t>
-  </si>
-  <si>
-    <t>NPN Vceo=40V, Ic=200mA, hfe=100@10mA</t>
-  </si>
-  <si>
-    <t>NPN Vceo=40V, Ic=1A, hfe=75@10mA</t>
-  </si>
-  <si>
-    <t>PNP Vceo=-40V, Ic=-200mA, hfe=100@10mA</t>
-  </si>
-  <si>
-    <t>NPN Vceo=40V, Ic=600mA, hfe=80@10mA</t>
-  </si>
-  <si>
-    <t>PNP Vceo=-40V, Ic=-600mA, hfe=50@10mA</t>
-  </si>
-  <si>
-    <t>PNP Vceo=-40V, Ic=-600mA, hfe=100@10mA</t>
-  </si>
-  <si>
-    <t>NPN Vceo=45V, Ic=100mA, hfe=110@2mA</t>
-  </si>
-  <si>
-    <t>PNP Vceo=-45V, Ic=100mA, hfe=110@2mA</t>
-  </si>
-  <si>
-    <t>BC550</t>
-  </si>
-  <si>
-    <t>N-JFET Vds=25V, Id=10mA, Vgs=-2.5V</t>
-  </si>
-  <si>
-    <t>N-JFET Vds=25V, Id=10mA, Vgs=-3.5V</t>
-  </si>
-  <si>
-    <t>N-FET Vds=25V, Id=10mA, Vgs=-4.5V</t>
-  </si>
-  <si>
-    <t>N-JFET</t>
-  </si>
-  <si>
-    <t>P-JFET</t>
-  </si>
-  <si>
-    <t>P-FET Vds=40V, Id=10mA, Vgs=0.8V to 4.5V</t>
-  </si>
-  <si>
-    <t>P-FET Vds=40V, Id=10mA, Vgs=0.5V to 4V</t>
-  </si>
-  <si>
-    <t>N-FET Vds=40V, Id=50mA, Vgs=-0.8V to -4V</t>
-  </si>
-  <si>
-    <t>MMBFJ201</t>
-  </si>
-  <si>
-    <t>N-FET Vds=40V, Id=50mA, Vgs=-0.3V to -1.5V</t>
-  </si>
-  <si>
-    <t>N-MOSFET Vds=60V, Id=200mA, Vgs=2.1V, Rds=1.2ohms</t>
-  </si>
-  <si>
-    <t>N-MOSFET Vds=60V, Id=115mA, Vgs=2.1V , Rds=1.2ohms</t>
-  </si>
-  <si>
-    <t>N-MOSFET</t>
-  </si>
-  <si>
     <t>TL072</t>
   </si>
   <si>
@@ -458,24 +276,6 @@
     <t>Alpha</t>
   </si>
   <si>
-    <t>J111</t>
-  </si>
-  <si>
-    <t>J112</t>
-  </si>
-  <si>
-    <t>J113</t>
-  </si>
-  <si>
-    <t>2n5484</t>
-  </si>
-  <si>
-    <t>2n5485</t>
-  </si>
-  <si>
-    <t>2n5486</t>
-  </si>
-  <si>
     <t>SF12020F-0202-20R-L-011</t>
   </si>
   <si>
@@ -584,18 +384,6 @@
     <t>Jack 1/8" TRS-B</t>
   </si>
   <si>
-    <t>Low Noise, High Gain, Use MMBT5089</t>
-  </si>
-  <si>
-    <t>Obsolete</t>
-  </si>
-  <si>
-    <t>High Current Gain, up to 1A collector use MMBTA14</t>
-  </si>
-  <si>
-    <t>High Current Gain, up to 800ma collector, use MMBTA63</t>
-  </si>
-  <si>
     <t>3PDT Footswitch Latching Solder Tabs</t>
   </si>
   <si>
@@ -617,9 +405,6 @@
     <t>9V Battery Clip</t>
   </si>
   <si>
-    <t>BS170</t>
-  </si>
-  <si>
     <t>LM321</t>
   </si>
   <si>
@@ -1095,75 +880,6 @@
   </si>
   <si>
     <t>MSS400-0001</t>
-  </si>
-  <si>
-    <t>MSS500-0001</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>Rectifier</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Diodes Inc</t>
-  </si>
-  <si>
-    <t>1N4001-T</t>
-  </si>
-  <si>
-    <t>DO-41</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>1.1V</t>
-  </si>
-  <si>
-    <t>30uA</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Rectifier Diode, 1A @ 1.1Vf, 50Vrrm, DO-41</t>
-  </si>
-  <si>
-    <t>621-1N4001</t>
-  </si>
-  <si>
-    <t>MSS500-0002</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>MSS500-0003</t>
-  </si>
-  <si>
-    <t>1N914</t>
-  </si>
-  <si>
-    <t>MSS500-0004</t>
-  </si>
-  <si>
-    <t>Rectron</t>
-  </si>
-  <si>
-    <t>1N4007-T</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>Rectifier Diode, 1A @ 1.1Vf, 1000Vrrm, DO-41</t>
-  </si>
-  <si>
-    <t>583-1N4007-T</t>
   </si>
   <si>
     <t>629-GRS401116</t>
@@ -1450,8 +1166,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1750,484 +1494,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G1" t="s">
-        <v>289</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>189</v>
-      </c>
-      <c r="I3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>189</v>
-      </c>
-      <c r="I6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" t="s">
-        <v>199</v>
-      </c>
-      <c r="D35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -2247,25 +1513,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -2273,408 +1539,408 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>226</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>220</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>231</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>234</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
       <c r="C31" t="s">
-        <v>236</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>237</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>238</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>239</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>243</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>246</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>247</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>248</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>272</v>
+        <v>201</v>
       </c>
       <c r="B43" t="s">
-        <v>270</v>
+        <v>199</v>
       </c>
       <c r="C43" t="s">
-        <v>271</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>273</v>
+        <v>202</v>
       </c>
       <c r="C44" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -2687,448 +1953,448 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>275</v>
+        <v>204</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>277</v>
+        <v>206</v>
       </c>
       <c r="C47" t="s">
-        <v>278</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>358</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C48" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D48" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E48" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F48" t="s">
-        <v>357</v>
+        <v>286</v>
       </c>
       <c r="G48" t="s">
-        <v>304</v>
+        <v>233</v>
       </c>
       <c r="H48" t="s">
-        <v>356</v>
+        <v>285</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>338</v>
+        <v>267</v>
       </c>
       <c r="J48" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K48" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="L48" t="s">
-        <v>355</v>
+        <v>284</v>
       </c>
       <c r="M48" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N48" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O48" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P48" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q48" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R48" t="s">
-        <v>354</v>
+        <v>283</v>
       </c>
       <c r="U48" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="V48" t="s">
-        <v>353</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>352</v>
+        <v>281</v>
       </c>
       <c r="B49" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D49" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E49" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F49" t="s">
-        <v>351</v>
+        <v>280</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>350</v>
+        <v>279</v>
       </c>
       <c r="J49" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K49" t="s">
-        <v>349</v>
+        <v>278</v>
       </c>
       <c r="L49" t="s">
-        <v>348</v>
+        <v>277</v>
       </c>
       <c r="M49" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N49" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O49" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P49" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q49" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R49" t="s">
-        <v>347</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>346</v>
+        <v>275</v>
       </c>
       <c r="B50" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C50" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D50" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E50" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>345</v>
+        <v>274</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>344</v>
+        <v>273</v>
       </c>
       <c r="J50" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K50" t="s">
-        <v>343</v>
+        <v>272</v>
       </c>
       <c r="L50" t="s">
-        <v>342</v>
+        <v>271</v>
       </c>
       <c r="M50" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N50" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O50" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P50" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q50" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R50" t="s">
-        <v>341</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>340</v>
+        <v>269</v>
       </c>
       <c r="B51" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D51" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E51" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F51" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>338</v>
+        <v>267</v>
       </c>
       <c r="J51" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K51" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="L51" t="s">
-        <v>337</v>
+        <v>266</v>
       </c>
       <c r="M51" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N51" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O51" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P51" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q51" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R51" t="s">
-        <v>336</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>335</v>
+        <v>264</v>
       </c>
       <c r="B52" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D52" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E52" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F52" t="s">
-        <v>334</v>
+        <v>263</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>333</v>
+        <v>262</v>
       </c>
       <c r="J52" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K52" t="s">
-        <v>332</v>
+        <v>261</v>
       </c>
       <c r="L52" t="s">
-        <v>331</v>
+        <v>260</v>
       </c>
       <c r="M52" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N52" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O52" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P52" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q52" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R52" t="s">
-        <v>330</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>329</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="C53" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D53" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E53" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="F53" t="s">
-        <v>325</v>
+        <v>254</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>324</v>
+        <v>253</v>
       </c>
       <c r="J53" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="K53" t="s">
-        <v>323</v>
+        <v>252</v>
       </c>
       <c r="L53" t="s">
-        <v>322</v>
+        <v>251</v>
       </c>
       <c r="M53" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="N53" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="O53" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="P53" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q53" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="R53" t="s">
-        <v>319</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="B54" t="s">
-        <v>308</v>
+        <v>237</v>
       </c>
       <c r="C54" t="s">
-        <v>317</v>
+        <v>246</v>
       </c>
       <c r="D54" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E54" t="s">
-        <v>306</v>
+        <v>235</v>
       </c>
       <c r="F54" t="s">
-        <v>316</v>
+        <v>245</v>
       </c>
       <c r="G54" t="s">
-        <v>304</v>
+        <v>233</v>
       </c>
       <c r="H54" t="s">
-        <v>315</v>
+        <v>244</v>
       </c>
       <c r="I54" t="s">
-        <v>314</v>
+        <v>243</v>
       </c>
       <c r="J54" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="L54" t="s">
-        <v>313</v>
+        <v>242</v>
       </c>
       <c r="M54" t="s">
-        <v>312</v>
+        <v>241</v>
       </c>
       <c r="N54" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="O54" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="P54" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q54" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="R54" t="s">
-        <v>311</v>
+        <v>240</v>
       </c>
       <c r="U54" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="V54" t="s">
-        <v>310</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>309</v>
+        <v>238</v>
       </c>
       <c r="B55" t="s">
-        <v>308</v>
+        <v>237</v>
       </c>
       <c r="C55" t="s">
-        <v>307</v>
+        <v>236</v>
       </c>
       <c r="D55" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E55" t="s">
-        <v>306</v>
+        <v>235</v>
       </c>
       <c r="F55" t="s">
-        <v>305</v>
+        <v>234</v>
       </c>
       <c r="G55" t="s">
-        <v>304</v>
+        <v>233</v>
       </c>
       <c r="H55" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
       <c r="I55" t="s">
-        <v>302</v>
+        <v>231</v>
       </c>
       <c r="J55" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="L55" t="s">
-        <v>301</v>
+        <v>230</v>
       </c>
       <c r="M55" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
       <c r="N55" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="O55" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="P55" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="Q55" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="R55" t="s">
-        <v>298</v>
+        <v>227</v>
       </c>
       <c r="U55" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="V55" t="s">
-        <v>297</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3137,179 +2403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="14" max="14" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="P1" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q1" s="1"/>
-      <c r="S1" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="T1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F2" t="s">
-        <v>373</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="O2" t="s">
-        <v>360</v>
-      </c>
-      <c r="P2" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>374</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="O3" t="s">
-        <v>360</v>
-      </c>
-      <c r="P3" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>376</v>
-      </c>
-      <c r="B4" t="s">
-        <v>360</v>
-      </c>
-      <c r="C4" t="s">
-        <v>361</v>
-      </c>
-      <c r="D4" t="s">
-        <v>362</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="P4" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="S4" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="T4" t="s">
-        <v>381</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
@@ -3336,28 +2430,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>214</v>
       </c>
       <c r="E1" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="G1" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
       <c r="H1" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
@@ -3365,676 +2459,676 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>282</v>
+        <v>211</v>
       </c>
       <c r="E4" t="s">
-        <v>281</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>208</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>267</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>268</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>269</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>442</v>
+        <v>348</v>
       </c>
       <c r="B33" t="s">
-        <v>441</v>
+        <v>347</v>
       </c>
       <c r="C33" t="s">
-        <v>440</v>
+        <v>346</v>
       </c>
       <c r="D33" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E33" t="s">
-        <v>424</v>
+        <v>330</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>439</v>
+        <v>345</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>413</v>
+        <v>319</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>438</v>
+        <v>344</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>437</v>
+        <v>343</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>436</v>
+        <v>342</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>435</v>
+        <v>341</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>434</v>
+        <v>340</v>
       </c>
       <c r="M33" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="P33" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="Q33" t="s">
-        <v>433</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>432</v>
+        <v>338</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>431</v>
+        <v>337</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>430</v>
+        <v>336</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>429</v>
+        <v>335</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>428</v>
+        <v>334</v>
       </c>
       <c r="E36" t="s">
-        <v>413</v>
+        <v>319</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>427</v>
+        <v>333</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>426</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>425</v>
+        <v>331</v>
       </c>
       <c r="E37" t="s">
-        <v>424</v>
+        <v>330</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>423</v>
+        <v>329</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="J37" t="s">
-        <v>422</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>421</v>
+        <v>327</v>
       </c>
       <c r="E38" t="s">
-        <v>420</v>
+        <v>326</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>419</v>
+        <v>325</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="J38" t="s">
-        <v>418</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>417</v>
+        <v>323</v>
       </c>
       <c r="E39" t="s">
-        <v>413</v>
+        <v>319</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>416</v>
+        <v>322</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>415</v>
+        <v>321</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>414</v>
+        <v>320</v>
       </c>
       <c r="E40" t="s">
-        <v>413</v>
+        <v>319</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>412</v>
+        <v>318</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>411</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>410</v>
+        <v>316</v>
       </c>
       <c r="E41" t="s">
-        <v>409</v>
+        <v>315</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="J41" t="s">
-        <v>408</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>407</v>
+        <v>313</v>
       </c>
       <c r="B42" t="s">
-        <v>406</v>
+        <v>312</v>
       </c>
       <c r="C42" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D42" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>405</v>
+        <v>311</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>404</v>
+        <v>310</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>403</v>
+        <v>309</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>402</v>
+        <v>308</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>401</v>
+        <v>307</v>
       </c>
       <c r="M42" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>400</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s">
-        <v>399</v>
+        <v>305</v>
       </c>
       <c r="C43" t="s">
-        <v>398</v>
+        <v>304</v>
       </c>
       <c r="D43" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="E43" t="s">
-        <v>397</v>
+        <v>303</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>396</v>
+        <v>302</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
-        <v>395</v>
+        <v>301</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>394</v>
+        <v>300</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>393</v>
+        <v>299</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>392</v>
+        <v>298</v>
       </c>
       <c r="M43" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="P43" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="Q43" t="s">
-        <v>391</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>390</v>
+        <v>296</v>
       </c>
       <c r="B44" t="s">
-        <v>389</v>
+        <v>295</v>
       </c>
       <c r="C44" t="s">
-        <v>296</v>
+        <v>225</v>
       </c>
       <c r="D44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44" t="s">
+        <v>294</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="E44" t="s">
-        <v>388</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
-        <v>386</v>
+        <v>292</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>385</v>
+        <v>291</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>384</v>
+        <v>290</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>383</v>
+        <v>289</v>
       </c>
       <c r="M44" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="P44" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="Q44" t="s">
-        <v>382</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4044,11 +3138,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -4060,25 +3154,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -4086,29 +3180,29 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>252</v>
+        <v>181</v>
       </c>
       <c r="I4" t="s">
         <v>6</v>
@@ -4116,10 +3210,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
@@ -4127,7 +3221,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>251</v>
+        <v>180</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -4135,7 +3229,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>253</v>
+        <v>182</v>
       </c>
       <c r="I7" t="s">
         <v>3</v>
@@ -4143,7 +3237,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>254</v>
+        <v>183</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
@@ -4151,7 +3245,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>255</v>
+        <v>184</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
@@ -4159,7 +3253,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>256</v>
+        <v>185</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -4167,7 +3261,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
@@ -4175,7 +3269,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>258</v>
+        <v>187</v>
       </c>
       <c r="I12" t="s">
         <v>9</v>
@@ -4183,7 +3277,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>259</v>
+        <v>188</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -4191,7 +3285,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>260</v>
+        <v>189</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
@@ -4199,7 +3293,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>261</v>
+        <v>190</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
@@ -4207,7 +3301,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>262</v>
+        <v>191</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
@@ -4215,7 +3309,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>263</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
         <v>15</v>
@@ -4223,7 +3317,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>264</v>
+        <v>193</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
@@ -4231,149 +3325,149 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>460</v>
+        <v>366</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>459</v>
+        <v>365</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>458</v>
+        <v>364</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>457</v>
+        <v>363</v>
       </c>
       <c r="K21" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="L21" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>456</v>
+        <v>362</v>
       </c>
       <c r="B22" t="s">
-        <v>450</v>
+        <v>356</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" t="s">
-        <v>449</v>
+        <v>355</v>
       </c>
       <c r="J22" t="s">
-        <v>455</v>
+        <v>361</v>
       </c>
       <c r="K22" t="s">
-        <v>454</v>
+        <v>360</v>
       </c>
       <c r="L22" t="s">
-        <v>446</v>
+        <v>352</v>
       </c>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>451</v>
+        <v>357</v>
       </c>
       <c r="B23" t="s">
-        <v>450</v>
+        <v>356</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" t="s">
-        <v>449</v>
+        <v>355</v>
       </c>
       <c r="J23" t="s">
-        <v>453</v>
+        <v>359</v>
       </c>
       <c r="K23" t="s">
-        <v>452</v>
+        <v>358</v>
       </c>
       <c r="L23" t="s">
-        <v>446</v>
+        <v>352</v>
       </c>
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>451</v>
+        <v>357</v>
       </c>
       <c r="B24" t="s">
-        <v>450</v>
+        <v>356</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" t="s">
-        <v>449</v>
+        <v>355</v>
       </c>
       <c r="J24" t="s">
-        <v>448</v>
+        <v>354</v>
       </c>
       <c r="K24" t="s">
-        <v>447</v>
+        <v>353</v>
       </c>
       <c r="L24" t="s">
-        <v>446</v>
+        <v>352</v>
       </c>
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>443</v>
+        <v>349</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="J25" t="s">
-        <v>445</v>
+        <v>351</v>
       </c>
       <c r="K25" t="s">
-        <v>444</v>
+        <v>350</v>
       </c>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>443</v>
+        <v>349</v>
       </c>
       <c r="E26" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>

</xml_diff>